<commit_message>
Created Schema (XSD/JSON) documents, and used them for validation in get pet by ID method
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/Data_PetStore.xlsx
+++ b/src/test/java/TestData/Data_PetStore.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MaheshStudy\BDD_DEMO\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9034D6-4B44-4865-8C05-C354C208E6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4CF3B1-3976-4BE1-8CBD-2778379521A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ADD_PET" sheetId="1" r:id="rId1"/>
-    <sheet name="GET_PET" sheetId="2" r:id="rId2"/>
+    <sheet name="PetStoreDetails" sheetId="3" r:id="rId1"/>
+    <sheet name="ADD_PET" sheetId="1" r:id="rId2"/>
+    <sheet name="GET_PET" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -50,12 +51,86 @@
         </r>
       </text>
     </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{D0E23A1F-ED20-46CD-A091-729C37E6A5A3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mahesh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+If multiple values separate them by ;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{9A3C56C1-6976-402D-AD0C-76C03885F4CD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mahesh:
+If multiple values separate them by ;</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mahesh</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8C9207DC-4749-40EE-84DC-03D42DA33165}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mahesh:
+Basis on this, get method will provide with either XML or JSON response body</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="67">
   <si>
     <t>Unique_Test_Case_ID</t>
   </si>
@@ -150,9 +225,6 @@
     <t>hold</t>
   </si>
   <si>
-    <t>TC_03_Get_Pet_From_Store_with_invalid_PetID_doesnt_exist</t>
-  </si>
-  <si>
     <t>MyDogPicURL1;MyDogPicURL2;MyDogPicURL3</t>
   </si>
   <si>
@@ -168,24 +240,6 @@
     <t>MandatoryURL_MyDogPicURL1</t>
   </si>
   <si>
-    <t>TC_03_Add_Pet_To_Store_XML_WithOnlyMandatoryFields</t>
-  </si>
-  <si>
-    <t>TC_01_Add_Pet_To_Store_XML_input_AllFieldsProvided</t>
-  </si>
-  <si>
-    <t>TC_02_Add_Pet_To_Store_Json_input_AllFieldsProvided</t>
-  </si>
-  <si>
-    <t>TC_05_Add_Pet_To_Store_XML_WithMultiplePicsAndTags</t>
-  </si>
-  <si>
-    <t>TC_06_Add_Pet_To_Store_JSON_WithMultiplePicsAndTags</t>
-  </si>
-  <si>
-    <t>TC_04_Add_Pet_To_Store_JSON_WithOnlyMandatoryFields</t>
-  </si>
-  <si>
     <t>Dog</t>
   </si>
   <si>
@@ -207,20 +261,292 @@
     <t>Domestic</t>
   </si>
   <si>
-    <t>TC_07_Add_Pet_Json_Invalid_Details_MissingHeader_accept</t>
-  </si>
-  <si>
-    <t>TC_08_Add_Pet_Json_Invalid_Details_MissingHeader_content-type</t>
-  </si>
-  <si>
-    <t>TC_09_Add_Pet_Json_Invalid_Details_wrong_PetStatus</t>
+    <t>USE_LATEST_FROM_DB</t>
+  </si>
+  <si>
+    <t>CREATE_NEW</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://petstore.swagger.io/</t>
+  </si>
+  <si>
+    <t>Pet Details</t>
+  </si>
+  <si>
+    <t>Mandatory Fields : Name and PhotoUrls</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Mandatory string value</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>photoUrls:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  array of strings</t>
+    </r>
+  </si>
+  <si>
+    <t>Add Pet service</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Optional Integer property
+1. If provided in payload while add service, same value will be returned on response   
+2. If not provided, service generates one and returns on response</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_01_Pet_In_Store_XML_input_AllFieldsProvided</t>
+  </si>
+  <si>
+    <t>TC_02_Pet_In_Store_Json_input_AllFieldsProvided</t>
+  </si>
+  <si>
+    <t>TC_03_Pet_In_Store_XML_WithOnlyMandatoryFields</t>
+  </si>
+  <si>
+    <t>TC_04_Pet_In_Store_JSON_WithOnlyMandatoryFields</t>
+  </si>
+  <si>
+    <t>TC_05_Pet_In_Store_XML_WithMultiplePicsAndTags</t>
+  </si>
+  <si>
+    <t>TC_06_Pet_In_Store_JSON_WithMultiplePicsAndTags</t>
+  </si>
+  <si>
+    <t>TC_07_Pet_In_Store_Json_Invalid_Details_MissingHeader_accept</t>
+  </si>
+  <si>
+    <t>TC_08_Pet_In_Store_Json_Invalid_Details_MissingHeader_content-type</t>
+  </si>
+  <si>
+    <t>TC_09_Pet_In_Store_Json_Invalid_Details_wrong_PetStatus</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>category:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Optional Object with property's
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> id :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> integer and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> string</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tags:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arrays of objects with property's
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> integer and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> string</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : String value 
+from Enum - available, pending, sold</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_03_Pet_In_Store_XML_with_invalid_PetID_doesnt_exist</t>
+  </si>
+  <si>
+    <t>TC_04_Pet_In_Store_JSON_with_invalid_PetID_doesnt_exist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +678,22 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -540,7 +882,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -655,8 +997,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -699,12 +1056,21 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -738,6 +1104,7 @@
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
@@ -759,6 +1126,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C503A6-1EE6-BFE4-3DA5-CE7CC3458AF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3905250" y="85725"/>
+          <a:ext cx="5686425" cy="5153025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1055,10 +1488,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1119F61-B5C1-4483-9E02-D5A67E7542CD}">
+  <dimension ref="A2:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:A10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CEDCB476-A224-4707-B1A1-FC124D16D7BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1068,7 +1583,7 @@
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
@@ -1128,7 +1643,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -1145,14 +1660,14 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
+      <c r="G2" t="s">
+        <v>44</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
@@ -1164,7 +1679,7 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
         <v>23</v>
@@ -1175,7 +1690,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1192,26 +1707,26 @@
       <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
+      <c r="G3" t="s">
+        <v>44</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
         <v>23</v>
@@ -1222,7 +1737,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -1240,10 +1755,10 @@
         <v>18</v>
       </c>
       <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
         <v>35</v>
-      </c>
-      <c r="K4" t="s">
-        <v>36</v>
       </c>
       <c r="O4">
         <v>200</v>
@@ -1251,7 +1766,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -1269,10 +1784,10 @@
         <v>25</v>
       </c>
       <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
         <v>35</v>
-      </c>
-      <c r="K5" t="s">
-        <v>36</v>
       </c>
       <c r="O5">
         <v>200</v>
@@ -1280,7 +1795,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -1297,26 +1812,26 @@
       <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="b">
-        <v>0</v>
+      <c r="G6" t="s">
+        <v>44</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
         <v>32</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>33</v>
-      </c>
-      <c r="M6" t="s">
-        <v>34</v>
       </c>
       <c r="N6" t="s">
         <v>23</v>
@@ -1327,7 +1842,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -1344,26 +1859,26 @@
       <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="b">
-        <v>0</v>
+      <c r="G7" t="s">
+        <v>44</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="M7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N7" t="s">
         <v>23</v>
@@ -1374,7 +1889,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -1385,8 +1900,8 @@
       <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="G8" t="b">
-        <v>0</v>
+      <c r="G8" t="s">
+        <v>44</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1415,7 +1930,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1426,8 +1941,8 @@
       <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="b">
-        <v>0</v>
+      <c r="G9" t="s">
+        <v>44</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1456,7 +1971,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -1473,8 +1988,8 @@
       <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="G10" t="b">
-        <v>0</v>
+      <c r="G10" t="s">
+        <v>44</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1507,12 +2022,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O4"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +2038,7 @@
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
@@ -1583,7 +2098,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -1600,14 +2115,14 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
+      <c r="G2" t="s">
+        <v>43</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
@@ -1619,7 +2134,7 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
         <v>23</v>
@@ -1630,7 +2145,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1647,26 +2162,26 @@
       <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
+      <c r="G3" t="s">
+        <v>43</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
         <v>23</v>
@@ -1677,22 +2192,22 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G4">
         <v>-1</v>
@@ -1719,10 +2234,58 @@
         <v>23</v>
       </c>
       <c r="O4">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5">
         <v>404</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>